<commit_message>
working on skill group class
</commit_message>
<xml_diff>
--- a/library.xlsx
+++ b/library.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User Library\Michael\OneDrive\Projects\Programming\Python\warhammer 40k stuff\Marine Story Generator\repo\Dynamic-Story-Generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User Library\Michael\Documents\Projects\Programming Projects\Python Projects\Dynamic Story Generator\Dynamic-Story-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1209" documentId="8_{66A03544-ADAD-4DA8-9080-FD09602E69E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7D788230-8D64-40DB-94A3-D75305CA78BF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7663D02-C379-4D86-AF2E-A2782F537580}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24210" windowHeight="9735" activeTab="1" xr2:uid="{6E3BC6EE-222B-4AE7-8B06-6583935631F3}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
     <sheet name="skills" sheetId="2" r:id="rId2"/>
+    <sheet name="SkillGroups" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="1977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="2042">
   <si>
     <t xml:space="preserve">Valerius </t>
   </si>
@@ -4810,55 +4811,28 @@
 at all, or if you fail by five or more degrees, contradict your orders entirely.</t>
   </si>
   <si>
-    <t>Common Lore (Adeptus Arbites)</t>
-  </si>
-  <si>
     <t>Knowledge of the various arms and sub-sects of the Arbites, including such things as their ranking structure and common procedures.</t>
   </si>
   <si>
-    <t>Common Lore (Administratum)</t>
-  </si>
-  <si>
     <t>Broad knowledge of the inner workings, rules and regulations of the Administratum. and common procedures.</t>
   </si>
   <si>
     <t>Understanding of the hierarchy of the Cult of the Emperor, its rankings, greetings and general practices. And common procedures.</t>
   </si>
   <si>
-    <t>Common Lore (Ecclesiarchy)</t>
-  </si>
-  <si>
-    <t>Common Lore (Imperial Creed)</t>
-  </si>
-  <si>
     <t>Knowledge of the rites and practices of the Imperial Cult, the most common observances to the Emperor and the most well-known saints.</t>
   </si>
   <si>
     <t>Basic information about the ranking systems, logistics and structure of the Imperial Guard as well as such things as their common practices, both tactical and strategic.</t>
   </si>
   <si>
-    <t>Common Lore (Imperial Guard)</t>
-  </si>
-  <si>
     <t>Knowledge of the sectors, segmentums and most wellknown worlds of the Imperium.</t>
   </si>
   <si>
-    <t>Common Lore (Imperium)</t>
-  </si>
-  <si>
-    <t>Common Lore (Tech)</t>
-  </si>
-  <si>
     <t>An understanding of simple litanies and rituals to sooth and appease machine spirits.</t>
   </si>
   <si>
     <t>Understanding of organised crime and sedition within the Imperium.</t>
-  </si>
-  <si>
-    <t>Common Lore (Underworld)</t>
-  </si>
-  <si>
-    <t>Common Lore (War)</t>
   </si>
   <si>
     <t>Knowledge of great battles, notable (and notorious) commanders and heroes, as well as famous stratagems.</t>
@@ -4897,12 +4871,6 @@
     <t>Intimidate is a character’s ability to frighten others into either doing what he tells them or giving up information. A character skilled in Intimidation can bully their way past guards, terrify locals into giving up their secrets, or even force foes to back down from a fi ght for fear of the consequences.</t>
   </si>
   <si>
-    <t>Linguistics covers all kinds of spoken and written languages, including codes, ciphers, and secret tongues. A character with the Linguistics Skill has learnt to speak, read, and write (if it has a written form) a particular language, code or cipher. No test is normally required to use Linguistics as it pertains to normal speaking, reading, or writing.</t>
-  </si>
-  <si>
-    <t>Linquistics</t>
-  </si>
-  <si>
     <t>Logic is the ability to think logically, solve puzzles and dissect information rationally and quickly. A character skilled in Logic can detect patterns where others cannot, see how each piece fi ts together into a whole and gather meaning from chaos. In addition to fi nding clues, solving riddles, or completing puzzles, Logic can also be used to help a character in games and endeavours where chance plays a large part such as gambling.</t>
   </si>
   <si>
@@ -5965,14 +5933,242 @@
     <t>Patronis</t>
   </si>
   <si>
-    <t>Commerce</t>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Archaic</t>
+  </si>
+  <si>
+    <t>Scholastic Lore grants the Explorer knowledge of a particularly complex or esoteric subject. A successful Skill Test allows him to recall necessary information or research a particular subject should appropriate reference material be readily available. Scholastic Lore grants a depth of knowledge far beyond that of Common Lore, requiring both experience and study to obtain.</t>
+  </si>
+  <si>
+    <t>Astromancy</t>
+  </si>
+  <si>
+    <t>Beasts</t>
+  </si>
+  <si>
+    <t>Bureaucracy</t>
+  </si>
+  <si>
+    <t>Chymistry</t>
+  </si>
+  <si>
+    <t>Cryptology</t>
+  </si>
+  <si>
+    <t>Heraldry</t>
+  </si>
+  <si>
+    <t>Imperial Warrants</t>
+  </si>
+  <si>
+    <t>Imperial Creed</t>
+  </si>
+  <si>
+    <t>Judgement</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Navis Nobilite</t>
+  </si>
+  <si>
+    <t>Numerology</t>
+  </si>
+  <si>
+    <t>Occult</t>
+  </si>
+  <si>
+    <t>Philosophy</t>
+  </si>
+  <si>
+    <t>Knowledge concerning the theories of thought, belief, existence, and other intangibles. As it also includes logic and debate, it may be used for argument or creating philosophical works.</t>
+  </si>
+  <si>
+    <t>Tactica Imperialis</t>
+  </si>
+  <si>
+    <t>The theories of the Tactica Imperialis, as well as other systems of troop deployment and battle techniques used by the Imperium. This knowledge may be used to devise a battle plan or deduce the likely flow of war fought by Imperial forces.</t>
+  </si>
+  <si>
+    <t>Common Lore</t>
+  </si>
+  <si>
+    <t>Adeptus Arbites</t>
+  </si>
+  <si>
+    <t>Administratum</t>
+  </si>
+  <si>
+    <t>Ecclesiarchy</t>
+  </si>
+  <si>
+    <t>Imperial Guard</t>
+  </si>
+  <si>
+    <t>Imperium</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>Underworld</t>
+  </si>
+  <si>
+    <t>War</t>
+  </si>
+  <si>
+    <t>A collection of acronyms, jargon, and procedural litanies used by the Adeptus Administratum. It should be noted that this language can be exceedingly longwinded.</t>
+  </si>
+  <si>
+    <t>An allegorical language of devotion and politics, it makes use of religious metaphors and passages of holy texts in archaic High Gothic.</t>
+  </si>
+  <si>
+    <t>Military</t>
+  </si>
+  <si>
+    <t>A selection of coded phrases, jargon, hand gestures, references to ancient battles, and a surprising number of terms for death.</t>
+  </si>
+  <si>
+    <t>Navigator</t>
+  </si>
+  <si>
+    <t>A number of archaic, dead tongues or dialects, now only know to the ancient Nobilite families that keep the old languages alive.</t>
+  </si>
+  <si>
+    <t>A prearranged series of code phrases and inflections intelligible only to those in the same vessel or fleet. Each trader eventually develops their own system of clandestine communication.</t>
+  </si>
+  <si>
+    <t>This coded binary cant includes high and low frequency sound waves and occasionally optical pulses.</t>
+  </si>
+  <si>
+    <t>Underdeck</t>
+  </si>
+  <si>
+    <t>A crude version of Low Gothic originating in the underhives, but migrated to the bilges and lower decks of most vessels; it incorporates a mishmash of colourful slang terms.</t>
+  </si>
+  <si>
+    <t>Though no human can hope to capture the subtle nuances and sub-tones of this extremely complex and ancient language, it is enough to make one’s meaning clear.</t>
+  </si>
+  <si>
+    <t>Explorator Binary</t>
+  </si>
+  <si>
+    <t>Very similar to Techna-Lingua, the binary language of the Explorator fleets has diverged from its parent tongue; the Mechanicus permits its use, but frowns on it for official discourse. Questors and other field operatives use it to keep conversations private from their planet-bound brethren.</t>
+  </si>
+  <si>
+    <t>High Gothic</t>
+  </si>
+  <si>
+    <t>The official language of the Imperium, used by Imperial officials, nobility, members of the Ecclesiarchy, and those involved in high-level negotiations.</t>
+  </si>
+  <si>
+    <t>Low Gothic</t>
+  </si>
+  <si>
+    <t>The common tongue of the Imperium, used by the countless billions of ordinary citizens.</t>
+  </si>
+  <si>
+    <t>The gutteral half-language of the Green Skins.</t>
+  </si>
+  <si>
+    <t>Techna-Lingua</t>
+  </si>
+  <si>
+    <t>The official language of the Adeptus Mechanicus, this binary language has been optimized for rapid communication of technical data and servitor commands.</t>
+  </si>
+  <si>
+    <t>Trader's Cant</t>
+  </si>
+  <si>
+    <t>Many Rogue Traders employ this language when dealing with their fellow traders, which allows for rapidfire negotiations and interchange.</t>
+  </si>
+  <si>
+    <t>Archaeologist</t>
+  </si>
+  <si>
+    <t>Used to locate, examine, and analyze ancient ruins and artefacts.</t>
+  </si>
+  <si>
+    <t>Armourer</t>
+  </si>
+  <si>
+    <t>Used to design, upgrade, and forge weaponry, from personal arms to starship batteries.</t>
+  </si>
+  <si>
+    <t>Astrographer</t>
+  </si>
+  <si>
+    <t>Used to create two- and three-dimensional representations of stellar locations and warp routes.</t>
+  </si>
+  <si>
+    <t>Chymist</t>
+  </si>
+  <si>
+    <t>Used to create poisons, drugs, and a wide variety of other compounds.</t>
+  </si>
+  <si>
+    <t>Cryptographer</t>
+  </si>
+  <si>
+    <t>Used to create or decode ciphers, codes and other puzzles.</t>
+  </si>
+  <si>
+    <t>Explorator</t>
+  </si>
+  <si>
+    <t>Used in the exploration of unknown stellar regions.</t>
+  </si>
+  <si>
+    <t>Linguist</t>
+  </si>
+  <si>
+    <t>Used to learn or decipher new languages, both spoken and written.</t>
+  </si>
+  <si>
+    <t>Remembrancer</t>
+  </si>
+  <si>
+    <t>Used to recount events in a variety of art forms, from sculpture to poetry.</t>
+  </si>
+  <si>
+    <t>Shipwright</t>
+  </si>
+  <si>
+    <t>Used to inscribe patterns, text, and art onto materials.</t>
+  </si>
+  <si>
+    <t>Soothsayer</t>
+  </si>
+  <si>
+    <t>Used to design, upgrade, and create voidcapable vessels.</t>
+  </si>
+  <si>
+    <t>Technomat</t>
+  </si>
+  <si>
+    <t>Used to “foretell” the future by a number of interpretative arts, though its effectiveness is suspect.</t>
+  </si>
+  <si>
+    <t>Trader</t>
+  </si>
+  <si>
+    <t>Used to maintain and repair technological devices, but through rote memorisation rather than true understanding.</t>
+  </si>
+  <si>
+    <t>Voidfarer</t>
+  </si>
+  <si>
+    <t>Used in the day-to-day operation, logistics, and defence of starships.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6026,6 +6222,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -6035,7 +6237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -6058,12 +6260,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6137,6 +6354,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7569,22 +7795,22 @@
         <v>1448</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>1624</v>
+        <v>1613</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>1693</v>
+        <v>1682</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>1719</v>
+        <v>1708</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>1848</v>
+        <v>1837</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>1898</v>
+        <v>1887</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>1899</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7629,22 +7855,22 @@
         <v>1449</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1625</v>
+        <v>1614</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>1694</v>
+        <v>1683</v>
       </c>
       <c r="S2" s="25" t="s">
-        <v>1720</v>
+        <v>1709</v>
       </c>
       <c r="T2" s="22" t="s">
-        <v>1849</v>
+        <v>1838</v>
       </c>
       <c r="U2" s="22" t="s">
-        <v>1944</v>
+        <v>1933</v>
       </c>
       <c r="V2" s="24" t="s">
-        <v>1947</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7689,22 +7915,22 @@
         <v>1450</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>1626</v>
+        <v>1615</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>1695</v>
+        <v>1684</v>
       </c>
       <c r="S3" s="25" t="s">
-        <v>1721</v>
+        <v>1710</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>1850</v>
+        <v>1839</v>
       </c>
       <c r="U3" s="25" t="s">
-        <v>1900</v>
+        <v>1889</v>
       </c>
       <c r="V3" s="22" t="s">
-        <v>1971</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7749,22 +7975,22 @@
         <v>1451</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1627</v>
+        <v>1616</v>
       </c>
       <c r="R4" s="21" t="s">
-        <v>1696</v>
+        <v>1685</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>1722</v>
+        <v>1711</v>
       </c>
       <c r="T4" s="22" t="s">
-        <v>1851</v>
+        <v>1840</v>
       </c>
       <c r="U4" s="22" t="s">
-        <v>1945</v>
+        <v>1934</v>
       </c>
       <c r="V4" s="24" t="s">
-        <v>1948</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7809,22 +8035,22 @@
         <v>1452</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>1628</v>
+        <v>1617</v>
       </c>
       <c r="R5" s="21" t="s">
-        <v>1697</v>
+        <v>1686</v>
       </c>
       <c r="S5" s="23" t="s">
-        <v>1723</v>
+        <v>1712</v>
       </c>
       <c r="T5" s="22" t="s">
-        <v>1852</v>
+        <v>1841</v>
       </c>
       <c r="U5" s="25" t="s">
-        <v>1901</v>
+        <v>1890</v>
       </c>
       <c r="V5" s="24" t="s">
-        <v>1949</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7869,22 +8095,22 @@
         <v>1453</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>1629</v>
+        <v>1618</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>1698</v>
+        <v>1687</v>
       </c>
       <c r="S6" s="25" t="s">
-        <v>1724</v>
+        <v>1713</v>
       </c>
       <c r="T6" s="25" t="s">
-        <v>1853</v>
+        <v>1842</v>
       </c>
       <c r="U6" s="25" t="s">
-        <v>1902</v>
+        <v>1891</v>
       </c>
       <c r="V6" s="24" t="s">
-        <v>1950</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7929,22 +8155,22 @@
         <v>1454</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>1630</v>
+        <v>1619</v>
       </c>
       <c r="R7" s="22" t="s">
-        <v>1699</v>
+        <v>1688</v>
       </c>
       <c r="S7" s="23" t="s">
-        <v>1725</v>
+        <v>1714</v>
       </c>
       <c r="T7" s="22" t="s">
-        <v>1854</v>
+        <v>1843</v>
       </c>
       <c r="U7" s="25" t="s">
-        <v>1903</v>
+        <v>1892</v>
       </c>
       <c r="V7" s="24" t="s">
-        <v>1951</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7989,22 +8215,22 @@
         <v>1455</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>1631</v>
+        <v>1620</v>
       </c>
       <c r="R8" s="22" t="s">
-        <v>1700</v>
+        <v>1689</v>
       </c>
       <c r="S8" s="25" t="s">
-        <v>1726</v>
+        <v>1715</v>
       </c>
       <c r="T8" s="25" t="s">
-        <v>1855</v>
+        <v>1844</v>
       </c>
       <c r="U8" s="25" t="s">
-        <v>1744</v>
+        <v>1733</v>
       </c>
       <c r="V8" s="24" t="s">
-        <v>1952</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="9" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8049,22 +8275,22 @@
         <v>1456</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>1632</v>
+        <v>1621</v>
       </c>
       <c r="R9" s="22" t="s">
-        <v>1701</v>
+        <v>1690</v>
       </c>
       <c r="S9" s="23" t="s">
-        <v>1727</v>
+        <v>1716</v>
       </c>
       <c r="T9" s="25" t="s">
-        <v>1856</v>
+        <v>1845</v>
       </c>
       <c r="U9" s="25" t="s">
-        <v>1904</v>
+        <v>1893</v>
       </c>
       <c r="V9" s="24" t="s">
-        <v>1953</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8106,22 +8332,22 @@
         <v>1457</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>1633</v>
+        <v>1622</v>
       </c>
       <c r="R10" s="22" t="s">
-        <v>1702</v>
+        <v>1691</v>
       </c>
       <c r="S10" s="25" t="s">
-        <v>1728</v>
+        <v>1717</v>
       </c>
       <c r="T10" s="25" t="s">
-        <v>1857</v>
+        <v>1846</v>
       </c>
       <c r="U10" s="25" t="s">
-        <v>1905</v>
+        <v>1894</v>
       </c>
       <c r="V10" s="24" t="s">
-        <v>1954</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8163,22 +8389,22 @@
         <v>1458</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>1634</v>
+        <v>1623</v>
       </c>
       <c r="R11" s="22" t="s">
-        <v>1703</v>
+        <v>1692</v>
       </c>
       <c r="S11" s="23" t="s">
-        <v>1729</v>
+        <v>1718</v>
       </c>
       <c r="T11" s="22" t="s">
-        <v>1858</v>
+        <v>1847</v>
       </c>
       <c r="U11" s="25" t="s">
-        <v>1906</v>
+        <v>1895</v>
       </c>
       <c r="V11" s="24" t="s">
-        <v>1955</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="12" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8217,22 +8443,22 @@
         <v>1459</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>1635</v>
+        <v>1624</v>
       </c>
       <c r="R12" s="24" t="s">
-        <v>1704</v>
+        <v>1693</v>
       </c>
       <c r="S12" s="23" t="s">
-        <v>1730</v>
+        <v>1719</v>
       </c>
       <c r="T12" s="25" t="s">
-        <v>1859</v>
+        <v>1848</v>
       </c>
       <c r="U12" s="25" t="s">
-        <v>1907</v>
+        <v>1896</v>
       </c>
       <c r="V12" s="24" t="s">
-        <v>1956</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="13" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8271,22 +8497,22 @@
         <v>1460</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>1636</v>
+        <v>1625</v>
       </c>
       <c r="R13" s="22" t="s">
-        <v>1705</v>
+        <v>1694</v>
       </c>
       <c r="S13" s="23" t="s">
-        <v>1731</v>
+        <v>1720</v>
       </c>
       <c r="T13" s="25" t="s">
-        <v>1860</v>
+        <v>1849</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>1908</v>
+        <v>1897</v>
       </c>
       <c r="V13" s="24" t="s">
-        <v>1957</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8325,22 +8551,22 @@
         <v>1463</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>1637</v>
+        <v>1626</v>
       </c>
       <c r="R14" s="22" t="s">
-        <v>1706</v>
+        <v>1695</v>
       </c>
       <c r="S14" s="23" t="s">
-        <v>1732</v>
+        <v>1721</v>
       </c>
       <c r="T14" s="25" t="s">
-        <v>1861</v>
+        <v>1850</v>
       </c>
       <c r="U14" s="25" t="s">
-        <v>1909</v>
+        <v>1898</v>
       </c>
       <c r="V14" s="24" t="s">
-        <v>1958</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="15" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8379,22 +8605,22 @@
         <v>1461</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>1638</v>
+        <v>1627</v>
       </c>
       <c r="R15" s="22" t="s">
-        <v>1707</v>
+        <v>1696</v>
       </c>
       <c r="S15" s="23" t="s">
-        <v>1733</v>
+        <v>1722</v>
       </c>
       <c r="T15" s="22" t="s">
-        <v>1862</v>
+        <v>1851</v>
       </c>
       <c r="U15" s="25" t="s">
-        <v>1910</v>
+        <v>1899</v>
       </c>
       <c r="V15" s="24" t="s">
-        <v>1959</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="16" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8433,22 +8659,22 @@
         <v>1462</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>1639</v>
+        <v>1628</v>
       </c>
       <c r="R16" s="22" t="s">
-        <v>1708</v>
+        <v>1697</v>
       </c>
       <c r="S16" s="25" t="s">
-        <v>1734</v>
+        <v>1723</v>
       </c>
       <c r="T16" s="25" t="s">
-        <v>1863</v>
+        <v>1852</v>
       </c>
       <c r="U16" s="25" t="s">
-        <v>1911</v>
+        <v>1900</v>
       </c>
       <c r="V16" s="24" t="s">
-        <v>1960</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="17" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8487,22 +8713,22 @@
         <v>1464</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>1640</v>
+        <v>1629</v>
       </c>
       <c r="R17" s="22" t="s">
-        <v>1709</v>
+        <v>1698</v>
       </c>
       <c r="S17" s="23" t="s">
-        <v>1735</v>
+        <v>1724</v>
       </c>
       <c r="T17" s="22" t="s">
-        <v>1864</v>
+        <v>1853</v>
       </c>
       <c r="U17" s="25" t="s">
-        <v>1912</v>
+        <v>1901</v>
       </c>
       <c r="V17" s="24" t="s">
-        <v>1961</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="18" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8541,22 +8767,22 @@
         <v>1465</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>1641</v>
+        <v>1630</v>
       </c>
       <c r="R18" s="22" t="s">
-        <v>1710</v>
+        <v>1699</v>
       </c>
       <c r="S18" s="25" t="s">
-        <v>1736</v>
+        <v>1725</v>
       </c>
       <c r="T18" s="22" t="s">
-        <v>1865</v>
+        <v>1854</v>
       </c>
       <c r="U18" s="25" t="s">
-        <v>1913</v>
+        <v>1902</v>
       </c>
       <c r="V18" s="24" t="s">
-        <v>1962</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="19" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8595,22 +8821,22 @@
         <v>1466</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>1642</v>
+        <v>1631</v>
       </c>
       <c r="R19" s="22" t="s">
-        <v>1711</v>
+        <v>1700</v>
       </c>
       <c r="S19" s="23" t="s">
-        <v>1737</v>
+        <v>1726</v>
       </c>
       <c r="T19" s="22" t="s">
-        <v>1866</v>
+        <v>1855</v>
       </c>
       <c r="U19" s="25" t="s">
-        <v>1914</v>
+        <v>1903</v>
       </c>
       <c r="V19" s="24" t="s">
-        <v>1963</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="20" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8649,22 +8875,22 @@
         <v>1467</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>1643</v>
+        <v>1632</v>
       </c>
       <c r="R20" s="24" t="s">
-        <v>1712</v>
+        <v>1701</v>
       </c>
       <c r="S20" s="23" t="s">
-        <v>1738</v>
+        <v>1727</v>
       </c>
       <c r="T20" s="25" t="s">
-        <v>1867</v>
+        <v>1856</v>
       </c>
       <c r="U20" s="25" t="s">
-        <v>1915</v>
+        <v>1904</v>
       </c>
       <c r="V20" s="24" t="s">
-        <v>1964</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="21" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8703,22 +8929,22 @@
         <v>1468</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>1644</v>
+        <v>1633</v>
       </c>
       <c r="R21" s="22" t="s">
-        <v>1713</v>
+        <v>1702</v>
       </c>
       <c r="S21" s="25" t="s">
-        <v>1739</v>
+        <v>1728</v>
       </c>
       <c r="T21" s="25" t="s">
-        <v>1868</v>
+        <v>1857</v>
       </c>
       <c r="U21" s="25" t="s">
-        <v>1916</v>
+        <v>1905</v>
       </c>
       <c r="V21" s="24" t="s">
-        <v>1965</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="22" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8757,22 +8983,22 @@
         <v>1469</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>1645</v>
+        <v>1634</v>
       </c>
       <c r="R22" s="22" t="s">
-        <v>1714</v>
+        <v>1703</v>
       </c>
       <c r="S22" s="23" t="s">
-        <v>1740</v>
+        <v>1729</v>
       </c>
       <c r="T22" s="22" t="s">
-        <v>1869</v>
+        <v>1858</v>
       </c>
       <c r="U22" s="25" t="s">
-        <v>1917</v>
+        <v>1906</v>
       </c>
       <c r="V22" s="24" t="s">
-        <v>1797</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="23" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8811,22 +9037,22 @@
         <v>1470</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>1646</v>
+        <v>1635</v>
       </c>
       <c r="R23" s="22" t="s">
-        <v>1715</v>
+        <v>1704</v>
       </c>
       <c r="S23" s="23" t="s">
-        <v>1741</v>
+        <v>1730</v>
       </c>
       <c r="T23" s="22" t="s">
-        <v>1870</v>
+        <v>1859</v>
       </c>
       <c r="U23" s="25" t="s">
-        <v>1918</v>
+        <v>1907</v>
       </c>
       <c r="V23" s="24" t="s">
-        <v>1975</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="24" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8865,19 +9091,19 @@
         <v>1471</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>1647</v>
+        <v>1636</v>
       </c>
       <c r="R24" s="22" t="s">
-        <v>1716</v>
+        <v>1705</v>
       </c>
       <c r="S24" s="23" t="s">
-        <v>1742</v>
+        <v>1731</v>
       </c>
       <c r="T24" s="22" t="s">
-        <v>1871</v>
+        <v>1860</v>
       </c>
       <c r="U24" s="25" t="s">
-        <v>1919</v>
+        <v>1908</v>
       </c>
       <c r="V24" s="24" t="s">
         <v>379</v>
@@ -8919,22 +9145,22 @@
         <v>1472</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>1648</v>
+        <v>1637</v>
       </c>
       <c r="R25" s="24" t="s">
-        <v>1717</v>
+        <v>1706</v>
       </c>
       <c r="S25" s="25" t="s">
-        <v>1743</v>
+        <v>1732</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>1872</v>
+        <v>1861</v>
       </c>
       <c r="U25" s="22" t="s">
-        <v>1946</v>
+        <v>1935</v>
       </c>
       <c r="V25" s="24" t="s">
-        <v>1974</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="26" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8973,22 +9199,22 @@
         <v>1473</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>1649</v>
+        <v>1638</v>
       </c>
       <c r="R26" s="24" t="s">
-        <v>1718</v>
+        <v>1707</v>
       </c>
       <c r="S26" s="23" t="s">
-        <v>1744</v>
+        <v>1733</v>
       </c>
       <c r="T26" s="22" t="s">
-        <v>1873</v>
+        <v>1862</v>
       </c>
       <c r="U26" s="25" t="s">
-        <v>1920</v>
+        <v>1909</v>
       </c>
       <c r="V26" s="24" t="s">
-        <v>1966</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="27" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9024,19 +9250,19 @@
         <v>1474</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>1650</v>
+        <v>1639</v>
       </c>
       <c r="S27" s="25" t="s">
-        <v>1745</v>
+        <v>1734</v>
       </c>
       <c r="T27" s="22" t="s">
-        <v>1874</v>
+        <v>1863</v>
       </c>
       <c r="U27" s="25" t="s">
-        <v>1921</v>
+        <v>1910</v>
       </c>
       <c r="V27" s="24" t="s">
-        <v>1967</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="28" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9072,19 +9298,19 @@
         <v>1475</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>1651</v>
+        <v>1640</v>
       </c>
       <c r="S28" s="23" t="s">
-        <v>1746</v>
+        <v>1735</v>
       </c>
       <c r="T28" s="22" t="s">
-        <v>1875</v>
+        <v>1864</v>
       </c>
       <c r="U28" s="25" t="s">
-        <v>1922</v>
+        <v>1911</v>
       </c>
       <c r="V28" s="24" t="s">
-        <v>1815</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="29" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9120,19 +9346,19 @@
         <v>1476</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>1652</v>
+        <v>1641</v>
       </c>
       <c r="S29" s="23" t="s">
-        <v>1747</v>
+        <v>1736</v>
       </c>
       <c r="T29" s="25" t="s">
-        <v>1876</v>
+        <v>1865</v>
       </c>
       <c r="U29" s="25" t="s">
-        <v>1923</v>
+        <v>1912</v>
       </c>
       <c r="V29" s="24" t="s">
-        <v>1972</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="30" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9168,19 +9394,19 @@
         <v>1477</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>1653</v>
+        <v>1642</v>
       </c>
       <c r="S30" s="25" t="s">
-        <v>1748</v>
+        <v>1737</v>
       </c>
       <c r="T30" s="25" t="s">
-        <v>1877</v>
+        <v>1866</v>
       </c>
       <c r="U30" s="25" t="s">
-        <v>1924</v>
+        <v>1913</v>
       </c>
       <c r="V30" s="24" t="s">
-        <v>1973</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="31" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9216,19 +9442,19 @@
         <v>1478</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>1654</v>
+        <v>1643</v>
       </c>
       <c r="S31" s="25" t="s">
-        <v>1749</v>
+        <v>1738</v>
       </c>
       <c r="T31" s="25" t="s">
-        <v>1878</v>
+        <v>1867</v>
       </c>
       <c r="U31" s="25" t="s">
-        <v>1925</v>
+        <v>1914</v>
       </c>
       <c r="V31" s="26" t="s">
-        <v>1968</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="32" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9264,19 +9490,19 @@
         <v>1479</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>1655</v>
+        <v>1644</v>
       </c>
       <c r="S32" s="23" t="s">
-        <v>1750</v>
+        <v>1739</v>
       </c>
       <c r="T32" s="22" t="s">
-        <v>1879</v>
+        <v>1868</v>
       </c>
       <c r="U32" s="25" t="s">
-        <v>1926</v>
+        <v>1915</v>
       </c>
       <c r="V32" s="24" t="s">
-        <v>1969</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="33" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9312,19 +9538,19 @@
         <v>1480</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>1656</v>
+        <v>1645</v>
       </c>
       <c r="S33" s="23" t="s">
-        <v>1751</v>
+        <v>1740</v>
       </c>
       <c r="T33" s="25" t="s">
-        <v>1880</v>
+        <v>1869</v>
       </c>
       <c r="U33" s="25" t="s">
-        <v>1927</v>
+        <v>1916</v>
       </c>
       <c r="V33" s="24" t="s">
-        <v>1970</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="34" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9360,16 +9586,16 @@
         <v>1481</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>1657</v>
+        <v>1646</v>
       </c>
       <c r="S34" s="25" t="s">
-        <v>1752</v>
+        <v>1741</v>
       </c>
       <c r="T34" s="25" t="s">
-        <v>1881</v>
+        <v>1870</v>
       </c>
       <c r="U34" s="25" t="s">
-        <v>1928</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="35" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9404,16 +9630,16 @@
         <v>1482</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>1658</v>
+        <v>1647</v>
       </c>
       <c r="S35" s="23" t="s">
-        <v>1753</v>
+        <v>1742</v>
       </c>
       <c r="T35" s="25" t="s">
-        <v>1882</v>
+        <v>1871</v>
       </c>
       <c r="U35" s="25" t="s">
-        <v>1929</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="36" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9447,16 +9673,16 @@
         <v>1483</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>1659</v>
+        <v>1648</v>
       </c>
       <c r="S36" s="23" t="s">
-        <v>1754</v>
+        <v>1743</v>
       </c>
       <c r="T36" s="25" t="s">
-        <v>1883</v>
+        <v>1872</v>
       </c>
       <c r="U36" s="25" t="s">
-        <v>1930</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="37" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9490,16 +9716,16 @@
         <v>1484</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>1660</v>
+        <v>1649</v>
       </c>
       <c r="S37" s="23" t="s">
-        <v>1755</v>
+        <v>1744</v>
       </c>
       <c r="T37" s="25" t="s">
-        <v>1884</v>
+        <v>1873</v>
       </c>
       <c r="U37" s="25" t="s">
-        <v>1931</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="38" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9533,16 +9759,16 @@
         <v>1485</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>1661</v>
+        <v>1650</v>
       </c>
       <c r="S38" s="25" t="s">
-        <v>1756</v>
+        <v>1745</v>
       </c>
       <c r="T38" s="25" t="s">
-        <v>1885</v>
+        <v>1874</v>
       </c>
       <c r="U38" s="25" t="s">
-        <v>1932</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9576,16 +9802,16 @@
         <v>1486</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>1662</v>
+        <v>1651</v>
       </c>
       <c r="S39" s="23" t="s">
-        <v>1757</v>
+        <v>1746</v>
       </c>
       <c r="T39" s="22" t="s">
-        <v>1886</v>
+        <v>1875</v>
       </c>
       <c r="U39" s="25" t="s">
-        <v>1933</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="40" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9619,16 +9845,16 @@
         <v>1487</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>1663</v>
+        <v>1652</v>
       </c>
       <c r="S40" s="25" t="s">
-        <v>1758</v>
+        <v>1747</v>
       </c>
       <c r="T40" s="22" t="s">
-        <v>1887</v>
+        <v>1876</v>
       </c>
       <c r="U40" s="25" t="s">
-        <v>1934</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="41" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9662,16 +9888,16 @@
         <v>1488</v>
       </c>
       <c r="Q41" s="4" t="s">
-        <v>1692</v>
+        <v>1681</v>
       </c>
       <c r="S41" s="23" t="s">
-        <v>1759</v>
+        <v>1748</v>
       </c>
       <c r="T41" s="22" t="s">
-        <v>1888</v>
+        <v>1877</v>
       </c>
       <c r="U41" s="25" t="s">
-        <v>1935</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="42" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9705,16 +9931,16 @@
         <v>1489</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>1664</v>
+        <v>1653</v>
       </c>
       <c r="S42" s="23" t="s">
-        <v>1760</v>
+        <v>1749</v>
       </c>
       <c r="T42" s="22" t="s">
-        <v>1889</v>
+        <v>1878</v>
       </c>
       <c r="U42" s="25" t="s">
-        <v>1936</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="43" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9748,16 +9974,16 @@
         <v>1490</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>1665</v>
+        <v>1654</v>
       </c>
       <c r="S43" s="23" t="s">
-        <v>1761</v>
+        <v>1750</v>
       </c>
       <c r="T43" s="22" t="s">
-        <v>1890</v>
+        <v>1879</v>
       </c>
       <c r="U43" s="25" t="s">
-        <v>1937</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="44" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9791,16 +10017,16 @@
         <v>1491</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>1666</v>
+        <v>1655</v>
       </c>
       <c r="S44" s="25" t="s">
-        <v>1762</v>
+        <v>1751</v>
       </c>
       <c r="T44" s="25" t="s">
-        <v>1891</v>
+        <v>1880</v>
       </c>
       <c r="U44" s="25" t="s">
-        <v>1938</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="45" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9834,16 +10060,16 @@
         <v>1492</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>1667</v>
+        <v>1656</v>
       </c>
       <c r="S45" s="25" t="s">
-        <v>1763</v>
+        <v>1752</v>
       </c>
       <c r="T45" s="25" t="s">
-        <v>1892</v>
+        <v>1881</v>
       </c>
       <c r="U45" s="25" t="s">
-        <v>1939</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="46" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9877,16 +10103,16 @@
         <v>1493</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>1668</v>
+        <v>1657</v>
       </c>
       <c r="S46" s="25" t="s">
-        <v>1764</v>
+        <v>1753</v>
       </c>
       <c r="T46" s="22" t="s">
-        <v>1893</v>
+        <v>1882</v>
       </c>
       <c r="U46" s="25" t="s">
-        <v>1940</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="47" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9920,16 +10146,16 @@
         <v>1494</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>1669</v>
+        <v>1658</v>
       </c>
       <c r="S47" s="25" t="s">
-        <v>1765</v>
+        <v>1754</v>
       </c>
       <c r="T47" s="25" t="s">
-        <v>1894</v>
+        <v>1883</v>
       </c>
       <c r="U47" s="25" t="s">
-        <v>1941</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="48" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9963,16 +10189,16 @@
         <v>1495</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>1670</v>
+        <v>1659</v>
       </c>
       <c r="S48" s="23" t="s">
-        <v>1766</v>
+        <v>1755</v>
       </c>
       <c r="T48" s="25" t="s">
-        <v>1895</v>
+        <v>1884</v>
       </c>
       <c r="U48" s="25" t="s">
-        <v>1942</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="49" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10005,16 +10231,16 @@
         <v>1496</v>
       </c>
       <c r="Q49" s="3" t="s">
-        <v>1671</v>
+        <v>1660</v>
       </c>
       <c r="S49" s="25" t="s">
-        <v>1767</v>
+        <v>1756</v>
       </c>
       <c r="T49" s="25" t="s">
-        <v>1838</v>
+        <v>1827</v>
       </c>
       <c r="U49" s="25" t="s">
-        <v>1943</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="50" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10048,13 +10274,13 @@
         <v>1497</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>1672</v>
+        <v>1661</v>
       </c>
       <c r="S50" s="25" t="s">
-        <v>1768</v>
+        <v>1757</v>
       </c>
       <c r="T50" s="25" t="s">
-        <v>1896</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="51" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10088,13 +10314,13 @@
         <v>1498</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>1673</v>
+        <v>1662</v>
       </c>
       <c r="S51" s="23" t="s">
-        <v>1769</v>
+        <v>1758</v>
       </c>
       <c r="T51" s="22" t="s">
-        <v>1897</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="52" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10128,10 +10354,10 @@
         <v>1499</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>1674</v>
+        <v>1663</v>
       </c>
       <c r="S52" s="25" t="s">
-        <v>1770</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="53" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10165,10 +10391,10 @@
         <v>1500</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>1675</v>
+        <v>1664</v>
       </c>
       <c r="S53" s="25" t="s">
-        <v>1771</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="54" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10202,10 +10428,10 @@
         <v>1501</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>1676</v>
+        <v>1665</v>
       </c>
       <c r="S54" s="23" t="s">
-        <v>1772</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="55" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10239,10 +10465,10 @@
         <v>1502</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>1677</v>
+        <v>1666</v>
       </c>
       <c r="S55" s="25" t="s">
-        <v>1773</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="56" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10276,10 +10502,10 @@
         <v>1503</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>1678</v>
+        <v>1667</v>
       </c>
       <c r="S56" s="25" t="s">
-        <v>1774</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="57" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10313,10 +10539,10 @@
         <v>1504</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>1679</v>
+        <v>1668</v>
       </c>
       <c r="S57" s="23" t="s">
-        <v>1775</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="58" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10350,7 +10576,7 @@
         <v>1505</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>1680</v>
+        <v>1669</v>
       </c>
       <c r="S58" s="23" t="s">
         <v>705</v>
@@ -10387,10 +10613,10 @@
         <v>1506</v>
       </c>
       <c r="Q59" s="3" t="s">
-        <v>1681</v>
+        <v>1670</v>
       </c>
       <c r="S59" s="25" t="s">
-        <v>1776</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="60" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10424,10 +10650,10 @@
         <v>1507</v>
       </c>
       <c r="Q60" s="3" t="s">
-        <v>1682</v>
+        <v>1671</v>
       </c>
       <c r="S60" s="25" t="s">
-        <v>1777</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="61" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10461,10 +10687,10 @@
         <v>1508</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>1683</v>
+        <v>1672</v>
       </c>
       <c r="S61" s="23" t="s">
-        <v>1778</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="62" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10498,10 +10724,10 @@
         <v>1509</v>
       </c>
       <c r="Q62" s="3" t="s">
-        <v>1684</v>
+        <v>1673</v>
       </c>
       <c r="S62" s="23" t="s">
-        <v>1779</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="63" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10535,10 +10761,10 @@
         <v>1510</v>
       </c>
       <c r="Q63" s="3" t="s">
-        <v>1685</v>
+        <v>1674</v>
       </c>
       <c r="S63" s="23" t="s">
-        <v>1780</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="64" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10572,10 +10798,10 @@
         <v>1511</v>
       </c>
       <c r="Q64" s="3" t="s">
-        <v>1686</v>
+        <v>1675</v>
       </c>
       <c r="S64" s="25" t="s">
-        <v>1781</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="65" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10608,10 +10834,10 @@
         <v>1512</v>
       </c>
       <c r="Q65" s="3" t="s">
-        <v>1687</v>
+        <v>1676</v>
       </c>
       <c r="S65" s="23" t="s">
-        <v>1782</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="66" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10645,10 +10871,10 @@
         <v>1513</v>
       </c>
       <c r="Q66" s="3" t="s">
-        <v>1688</v>
+        <v>1677</v>
       </c>
       <c r="S66" s="25" t="s">
-        <v>1708</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="67" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10680,7 +10906,7 @@
         <v>1514</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>1689</v>
+        <v>1678</v>
       </c>
       <c r="S67" s="25" t="s">
         <v>65</v>
@@ -10712,10 +10938,10 @@
         <v>988</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>1690</v>
+        <v>1679</v>
       </c>
       <c r="S68" s="23" t="s">
-        <v>1783</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="69" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10745,10 +10971,10 @@
         <v>1013</v>
       </c>
       <c r="Q69" s="3" t="s">
-        <v>1691</v>
+        <v>1680</v>
       </c>
       <c r="S69" s="23" t="s">
-        <v>1784</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="70" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10778,7 +11004,7 @@
         <v>989</v>
       </c>
       <c r="S70" s="25" t="s">
-        <v>1785</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="71" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10808,7 +11034,7 @@
         <v>1014</v>
       </c>
       <c r="S71" s="23" t="s">
-        <v>1786</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="72" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10839,7 +11065,7 @@
         <v>990</v>
       </c>
       <c r="S72" s="25" t="s">
-        <v>1787</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="73" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10870,7 +11096,7 @@
         <v>991</v>
       </c>
       <c r="S73" s="25" t="s">
-        <v>1788</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="74" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10901,7 +11127,7 @@
         <v>992</v>
       </c>
       <c r="S74" s="25" t="s">
-        <v>1789</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="75" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10932,7 +11158,7 @@
         <v>993</v>
       </c>
       <c r="S75" s="23" t="s">
-        <v>1790</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="76" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10963,7 +11189,7 @@
         <v>994</v>
       </c>
       <c r="S76" s="25" t="s">
-        <v>1791</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="77" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10994,7 +11220,7 @@
         <v>995</v>
       </c>
       <c r="S77" s="23" t="s">
-        <v>1846</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="78" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11025,7 +11251,7 @@
         <v>1015</v>
       </c>
       <c r="S78" s="25" t="s">
-        <v>1847</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="79" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11056,7 +11282,7 @@
         <v>1016</v>
       </c>
       <c r="S79" s="25" t="s">
-        <v>1792</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="80" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11087,7 +11313,7 @@
         <v>996</v>
       </c>
       <c r="S80" s="25" t="s">
-        <v>1793</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="81" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11118,7 +11344,7 @@
         <v>1017</v>
       </c>
       <c r="S81" s="23" t="s">
-        <v>1794</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="82" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11149,7 +11375,7 @@
         <v>997</v>
       </c>
       <c r="S82" s="23" t="s">
-        <v>1795</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="83" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11178,7 +11404,7 @@
         <v>998</v>
       </c>
       <c r="S83" s="23" t="s">
-        <v>1796</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="84" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11207,7 +11433,7 @@
         <v>999</v>
       </c>
       <c r="S84" s="23" t="s">
-        <v>1797</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="85" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11236,7 +11462,7 @@
         <v>1000</v>
       </c>
       <c r="S85" s="23" t="s">
-        <v>1798</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="86" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11265,7 +11491,7 @@
         <v>1001</v>
       </c>
       <c r="S86" s="23" t="s">
-        <v>1799</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="87" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11294,7 +11520,7 @@
         <v>1002</v>
       </c>
       <c r="S87" s="23" t="s">
-        <v>1800</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="88" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11323,7 +11549,7 @@
         <v>1018</v>
       </c>
       <c r="S88" s="23" t="s">
-        <v>1801</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="89" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11381,7 +11607,7 @@
         <v>1003</v>
       </c>
       <c r="S90" s="23" t="s">
-        <v>1802</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="91" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11410,7 +11636,7 @@
         <v>1004</v>
       </c>
       <c r="S91" s="23" t="s">
-        <v>1803</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="92" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11439,7 +11665,7 @@
         <v>1005</v>
       </c>
       <c r="S92" s="23" t="s">
-        <v>1804</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="93" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11468,7 +11694,7 @@
         <v>1020</v>
       </c>
       <c r="S93" s="23" t="s">
-        <v>1805</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="94" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11497,7 +11723,7 @@
         <v>1006</v>
       </c>
       <c r="S94" s="23" t="s">
-        <v>1806</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="95" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11526,7 +11752,7 @@
         <v>1007</v>
       </c>
       <c r="S95" s="25" t="s">
-        <v>1807</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="96" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11555,7 +11781,7 @@
         <v>1021</v>
       </c>
       <c r="S96" s="25" t="s">
-        <v>1808</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="97" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11584,7 +11810,7 @@
         <v>1022</v>
       </c>
       <c r="S97" s="25" t="s">
-        <v>1809</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="98" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11613,7 +11839,7 @@
         <v>1023</v>
       </c>
       <c r="S98" s="25" t="s">
-        <v>1810</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="99" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11642,7 +11868,7 @@
         <v>1008</v>
       </c>
       <c r="S99" s="23" t="s">
-        <v>1811</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="100" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11671,7 +11897,7 @@
         <v>1009</v>
       </c>
       <c r="S100" s="23" t="s">
-        <v>1812</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="101" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11700,7 +11926,7 @@
         <v>1024</v>
       </c>
       <c r="S101" s="23" t="s">
-        <v>1813</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="102" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11729,7 +11955,7 @@
         <v>1025</v>
       </c>
       <c r="S102" s="23" t="s">
-        <v>1814</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="103" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11758,7 +11984,7 @@
         <v>1026</v>
       </c>
       <c r="S103" s="25" t="s">
-        <v>1815</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="104" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11787,7 +12013,7 @@
         <v>1027</v>
       </c>
       <c r="S104" s="25" t="s">
-        <v>1816</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="105" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11816,7 +12042,7 @@
         <v>1010</v>
       </c>
       <c r="S105" s="23" t="s">
-        <v>1817</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="106" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11845,7 +12071,7 @@
         <v>1011</v>
       </c>
       <c r="S106" s="23" t="s">
-        <v>1818</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="107" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11874,7 +12100,7 @@
         <v>969</v>
       </c>
       <c r="S107" s="23" t="s">
-        <v>1819</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="108" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11900,7 +12126,7 @@
       <c r="L108" s="9"/>
       <c r="M108" s="17"/>
       <c r="S108" s="23" t="s">
-        <v>1820</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="109" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11926,7 +12152,7 @@
       <c r="L109" s="17"/>
       <c r="M109" s="9"/>
       <c r="S109" s="23" t="s">
-        <v>1821</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="110" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11951,7 +12177,7 @@
       <c r="L110" s="9"/>
       <c r="M110" s="9"/>
       <c r="S110" s="23" t="s">
-        <v>1822</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="111" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11977,7 +12203,7 @@
       <c r="L111" s="9"/>
       <c r="M111" s="17"/>
       <c r="S111" s="23" t="s">
-        <v>1823</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="112" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12002,7 +12228,7 @@
       <c r="L112" s="9"/>
       <c r="M112" s="17"/>
       <c r="S112" s="23" t="s">
-        <v>1824</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="113" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12027,7 +12253,7 @@
       <c r="L113" s="17"/>
       <c r="M113" s="17"/>
       <c r="S113" s="23" t="s">
-        <v>1825</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="114" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12052,7 +12278,7 @@
       <c r="L114" s="9"/>
       <c r="M114" s="17"/>
       <c r="S114" s="23" t="s">
-        <v>1826</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="115" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12077,7 +12303,7 @@
       <c r="L115" s="9"/>
       <c r="M115" s="17"/>
       <c r="S115" s="23" t="s">
-        <v>1827</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="116" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12102,7 +12328,7 @@
       <c r="L116" s="9"/>
       <c r="M116" s="9"/>
       <c r="S116" s="25" t="s">
-        <v>1828</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="117" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12127,7 +12353,7 @@
       <c r="L117" s="9"/>
       <c r="M117" s="17"/>
       <c r="S117" s="23" t="s">
-        <v>1829</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="118" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12152,7 +12378,7 @@
       <c r="L118" s="9"/>
       <c r="M118" s="17"/>
       <c r="S118" s="23" t="s">
-        <v>1830</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="119" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12177,7 +12403,7 @@
       <c r="L119" s="9"/>
       <c r="M119" s="17"/>
       <c r="S119" s="23" t="s">
-        <v>1831</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="120" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12202,7 +12428,7 @@
       <c r="L120" s="9"/>
       <c r="M120" s="9"/>
       <c r="S120" s="25" t="s">
-        <v>1832</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="121" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12227,7 +12453,7 @@
       <c r="L121" s="9"/>
       <c r="M121" s="9"/>
       <c r="S121" s="23" t="s">
-        <v>1833</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="122" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12252,7 +12478,7 @@
       <c r="L122" s="9"/>
       <c r="M122" s="9"/>
       <c r="S122" s="23" t="s">
-        <v>1834</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="123" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12277,7 +12503,7 @@
       <c r="L123" s="9"/>
       <c r="M123" s="9"/>
       <c r="S123" s="23" t="s">
-        <v>1835</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="124" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12302,7 +12528,7 @@
       <c r="L124" s="9"/>
       <c r="M124" s="9"/>
       <c r="S124" s="25" t="s">
-        <v>1836</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="125" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12327,7 +12553,7 @@
       <c r="L125" s="9"/>
       <c r="M125" s="17"/>
       <c r="S125" s="23" t="s">
-        <v>1837</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="126" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12352,7 +12578,7 @@
       <c r="L126" s="9"/>
       <c r="M126" s="17"/>
       <c r="S126" s="25" t="s">
-        <v>1838</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="127" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12377,7 +12603,7 @@
       <c r="L127" s="9"/>
       <c r="M127" s="9"/>
       <c r="S127" s="23" t="s">
-        <v>1839</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="128" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12402,7 +12628,7 @@
       <c r="L128" s="17"/>
       <c r="M128" s="9"/>
       <c r="S128" s="23" t="s">
-        <v>1840</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="129" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12427,7 +12653,7 @@
       <c r="L129" s="17"/>
       <c r="M129" s="17"/>
       <c r="S129" s="23" t="s">
-        <v>1841</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="130" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12452,7 +12678,7 @@
       <c r="L130" s="17"/>
       <c r="M130" s="17"/>
       <c r="S130" s="23" t="s">
-        <v>1842</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="131" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12477,7 +12703,7 @@
       <c r="L131" s="17"/>
       <c r="M131" s="17"/>
       <c r="S131" s="23" t="s">
-        <v>1843</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="132" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12502,7 +12728,7 @@
       <c r="L132" s="17"/>
       <c r="M132" s="17"/>
       <c r="S132" s="25" t="s">
-        <v>1844</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="133" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12527,7 +12753,7 @@
       <c r="L133" s="17"/>
       <c r="M133" s="17"/>
       <c r="S133" s="25" t="s">
-        <v>1845</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="134" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15334,10 +15560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3924F359-4018-4843-8FA7-64222961FF74}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="A53" sqref="A53:D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15569,7 +15795,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>1610</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -15583,7 +15809,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>1611</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -15597,7 +15823,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>1612</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -15611,7 +15837,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>1613</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -15625,7 +15851,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>1614</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -15639,7 +15865,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>1615</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -15653,7 +15879,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>1616</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -15703,7 +15929,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>1617</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -15717,7 +15943,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>1618</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -15731,7 +15957,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>1619</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -15781,7 +16007,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>1622</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -15795,7 +16021,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>1623</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -16027,157 +16253,960 @@
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>1592</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>1593</v>
-      </c>
+      <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>1594</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>1595</v>
-      </c>
+      <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>1597</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>1596</v>
-      </c>
+      <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>1598</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>1599</v>
-      </c>
+      <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>1601</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>1600</v>
-      </c>
+      <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>1603</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>1602</v>
-      </c>
+      <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>1604</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>1605</v>
-      </c>
+      <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>1607</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>1606</v>
-      </c>
+      <c r="D60" s="7"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>1608</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>1609</v>
-      </c>
+      <c r="D61" s="7"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>1621</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>1620</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>1976</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1526</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
+      <c r="D62" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D0369F-FED3-4742-B96E-6404388CD5DB}">
+  <dimension ref="A1:E53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1517</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D2" s="29">
+        <v>0</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>1968</v>
+      </c>
+      <c r="D3" s="29">
+        <v>0</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>1970</v>
+      </c>
+      <c r="D5" s="29">
+        <v>0</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>1971</v>
+      </c>
+      <c r="D6" s="29">
+        <v>0</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>1972</v>
+      </c>
+      <c r="D7" s="29">
+        <v>0</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>1973</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>1974</v>
+      </c>
+      <c r="D9" s="29">
+        <v>0</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>1975</v>
+      </c>
+      <c r="D10" s="29">
+        <v>0</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D11" s="29">
+        <v>0</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>1978</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>1979</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>1980</v>
+      </c>
+      <c r="D15" s="29">
+        <v>0</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D16" s="29">
+        <v>0</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>1983</v>
+      </c>
+      <c r="D17" s="29">
+        <v>0</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D18" s="29">
+        <v>0</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>1987</v>
+      </c>
+      <c r="D19" s="29">
+        <v>0</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>1988</v>
+      </c>
+      <c r="D20" s="29">
+        <v>0</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>1975</v>
+      </c>
+      <c r="D21" s="29">
+        <v>0</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>1989</v>
+      </c>
+      <c r="D22" s="29">
+        <v>0</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>1990</v>
+      </c>
+      <c r="D23" s="29">
+        <v>0</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>1991</v>
+      </c>
+      <c r="D24" s="29">
+        <v>0</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D25" s="29">
+        <v>0</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>1993</v>
+      </c>
+      <c r="D26" s="29">
+        <v>0</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>1987</v>
+      </c>
+      <c r="D27" s="29">
+        <v>0</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>1988</v>
+      </c>
+      <c r="D28" s="29">
+        <v>0</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>1996</v>
+      </c>
+      <c r="D29" s="29">
+        <v>0</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>1998</v>
+      </c>
+      <c r="D30" s="29">
+        <v>0</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="D31" s="29">
+        <v>0</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="27" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>1991</v>
+      </c>
+      <c r="D32" s="29">
+        <v>0</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D33" s="29">
+        <v>0</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="27" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D34" s="29">
+        <v>0</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D35" s="29">
+        <v>0</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>2007</v>
+      </c>
+      <c r="D36" s="29">
+        <v>0</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="27" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D37" s="29">
+        <v>0</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D38" s="29">
+        <v>0</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="27" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>2012</v>
+      </c>
+      <c r="D39" s="29">
+        <v>0</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="27" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>2014</v>
+      </c>
+      <c r="D40" s="29">
+        <v>0</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>2016</v>
+      </c>
+      <c r="D41" s="29">
+        <v>0</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>2018</v>
+      </c>
+      <c r="D42" s="29">
+        <v>0</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>2020</v>
+      </c>
+      <c r="D43" s="29">
+        <v>0</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>2022</v>
+      </c>
+      <c r="D44" s="29">
+        <v>0</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>2024</v>
+      </c>
+      <c r="D45" s="29">
+        <v>0</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>2026</v>
+      </c>
+      <c r="D46" s="29">
+        <v>0</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>2028</v>
+      </c>
+      <c r="D47" s="29">
+        <v>0</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>2030</v>
+      </c>
+      <c r="D48" s="29">
+        <v>0</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D49" s="29">
+        <v>0</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>2034</v>
+      </c>
+      <c r="D50" s="29">
+        <v>0</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>2036</v>
+      </c>
+      <c r="D51" s="29">
+        <v>0</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>2038</v>
+      </c>
+      <c r="D52" s="29">
+        <v>0</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="27" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B53" s="27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>2040</v>
+      </c>
+      <c r="D53" s="29">
+        <v>0</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working out the bugs with the AutoMaker Method. -MGC
</commit_message>
<xml_diff>
--- a/library.xlsx
+++ b/library.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User Library\Michael\Documents\Projects\Programming Projects\Python Projects\Dynamic Story Generator\Dynamic-Story-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7663D02-C379-4D86-AF2E-A2782F537580}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D5CB32-1092-4438-B360-D4B4ACC5B077}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24210" windowHeight="9735" activeTab="1" xr2:uid="{6E3BC6EE-222B-4AE7-8B06-6583935631F3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24210" windowHeight="9735" activeTab="3" xr2:uid="{6E3BC6EE-222B-4AE7-8B06-6583935631F3}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
     <sheet name="skills" sheetId="2" r:id="rId2"/>
     <sheet name="SkillGroups" sheetId="3" r:id="rId3"/>
+    <sheet name="weapons" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="2042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="2118">
   <si>
     <t xml:space="preserve">Valerius </t>
   </si>
@@ -6162,6 +6163,234 @@
   </si>
   <si>
     <t>Used in the day-to-day operation, logistics, and defence of starships.</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>RoF</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Pen</t>
+  </si>
+  <si>
+    <t>Clip</t>
+  </si>
+  <si>
+    <t>Reload</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Archeotech Laspistol</t>
+  </si>
+  <si>
+    <t>las</t>
+  </si>
+  <si>
+    <t>Pistol</t>
+  </si>
+  <si>
+    <t>S/3/-</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>Accurate, Reliable</t>
+  </si>
+  <si>
+    <t>Belasco Dueling Pistol</t>
+  </si>
+  <si>
+    <t>Hellpistol (Lucius)</t>
+  </si>
+  <si>
+    <t>Hellgun (lucius)</t>
+  </si>
+  <si>
+    <t>Las Gauntlets</t>
+  </si>
+  <si>
+    <t>Lascarbine (locke)</t>
+  </si>
+  <si>
+    <t>Lasgun</t>
+  </si>
+  <si>
+    <t>Laspistol</t>
+  </si>
+  <si>
+    <t>Long-las</t>
+  </si>
+  <si>
+    <t>Man Portable Lascannon</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>Heavy</t>
+  </si>
+  <si>
+    <t>S/-/-</t>
+  </si>
+  <si>
+    <t>S/2/-</t>
+  </si>
+  <si>
+    <t>S/4/-</t>
+  </si>
+  <si>
+    <t>4-13</t>
+  </si>
+  <si>
+    <t>Damage Type</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>6-15</t>
+  </si>
+  <si>
+    <t>5-14</t>
+  </si>
+  <si>
+    <t>3-12</t>
+  </si>
+  <si>
+    <t>15-60</t>
+  </si>
+  <si>
+    <t>2 full</t>
+  </si>
+  <si>
+    <t>Accurate</t>
+  </si>
+  <si>
+    <t>Reliable</t>
+  </si>
+  <si>
+    <t>Autogun</t>
+  </si>
+  <si>
+    <t>Autopistol</t>
+  </si>
+  <si>
+    <t>Hand Cannon</t>
+  </si>
+  <si>
+    <t>Heavy Stubber (orthlack)</t>
+  </si>
+  <si>
+    <t>Heavy Stubber (Ursid)</t>
+  </si>
+  <si>
+    <t>Naval Pistol (Mars)</t>
+  </si>
+  <si>
+    <t>Naval Shotcannon</t>
+  </si>
+  <si>
+    <t>Pump-Action Shotgun</t>
+  </si>
+  <si>
+    <t>Shotgun</t>
+  </si>
+  <si>
+    <t>Shotgun Pistol</t>
+  </si>
+  <si>
+    <t>Stub Automatic</t>
+  </si>
+  <si>
+    <t>Stub Revolver</t>
+  </si>
+  <si>
+    <t>Solid Projectile</t>
+  </si>
+  <si>
+    <t>Boltgun (Locke)</t>
+  </si>
+  <si>
+    <t>Bolt Pistol (Ceres)</t>
+  </si>
+  <si>
+    <t>Storm Bolter (Mars)</t>
+  </si>
+  <si>
+    <t>Heavy Bolter (Solar)</t>
+  </si>
+  <si>
+    <t>Bolt Weapon</t>
+  </si>
+  <si>
+    <t>Melta Weapons</t>
+  </si>
+  <si>
+    <t>Inferno Pistol (Mars)</t>
+  </si>
+  <si>
+    <t>Meltagun (Mars)</t>
+  </si>
+  <si>
+    <t>Meltagun (Mexoa)</t>
+  </si>
+  <si>
+    <t>Thermal Lance (Mars)</t>
+  </si>
+  <si>
+    <t>Multi-Melta (Mars)</t>
+  </si>
+  <si>
+    <t>S/3/10</t>
+  </si>
+  <si>
+    <t>S/-/6</t>
+  </si>
+  <si>
+    <t>-/-/10</t>
+  </si>
+  <si>
+    <t>S/2/4</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>Explosive</t>
+  </si>
+  <si>
+    <t>6-24</t>
+  </si>
+  <si>
+    <t>4-22</t>
+  </si>
+  <si>
+    <t>10-28</t>
+  </si>
+  <si>
+    <t>9-45</t>
   </si>
 </sst>
 </file>
@@ -6280,7 +6509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6363,6 +6592,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -15562,7 +15794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3924F359-4018-4843-8FA7-64222961FF74}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A53" sqref="A53:D63"/>
     </sheetView>
   </sheetViews>
@@ -16292,7 +16524,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17209,4 +17441,918 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F23AD-430A-455E-A79E-A746A5FB4081}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2042</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2043</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2044</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2045</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2047</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2075</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2048</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2049</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2050</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2051</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D2">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>2074</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2057</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2058</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2059</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D3">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>2077</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2057</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2082</v>
+      </c>
+      <c r="L3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2072</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>2078</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2081</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2061</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D5">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>2078</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2081</v>
+      </c>
+      <c r="L5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2062</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2073</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>2078</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2057</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2083</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2063</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2069</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2072</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>2074</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>2081</v>
+      </c>
+      <c r="K7" t="s">
+        <v>2083</v>
+      </c>
+      <c r="L7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2064</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2069</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>2074</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s">
+        <v>2057</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2083</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2065</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>2079</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>30</v>
+      </c>
+      <c r="J9" t="s">
+        <v>2057</v>
+      </c>
+      <c r="K9" t="s">
+        <v>2083</v>
+      </c>
+      <c r="L9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2066</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2069</v>
+      </c>
+      <c r="D10">
+        <v>150</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>2074</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>40</v>
+      </c>
+      <c r="J10" t="s">
+        <v>2057</v>
+      </c>
+      <c r="K10" t="s">
+        <v>2058</v>
+      </c>
+      <c r="L10">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2067</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D11">
+        <v>300</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>2080</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2081</v>
+      </c>
+      <c r="L11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D12">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2108</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>2074</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2085</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2109</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>2079</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2086</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D14">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>2078</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2087</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D15">
+        <v>120</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>2110</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>2077</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2088</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D16">
+        <v>120</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>2077</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2089</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>2078</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2090</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D18">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>2114</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D19">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>2078</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D20">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>2078</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>2078</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D22">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>2074</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D23">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>2074</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2097</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D24">
+        <v>90</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2111</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>2077</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2098</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D25">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2072</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>2077</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2099</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D26">
+        <v>90</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2111</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>2077</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D27">
+        <v>120</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>2110</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>2115</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2103</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2102</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>2116</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2104</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2102</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D29">
+        <v>20</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>2116</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2105</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2102</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>2116</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2106</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2102</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>2116</v>
+      </c>
+      <c r="G31" s="31" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2107</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2102</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D32">
+        <v>60</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F32" s="31" t="s">
+        <v>2117</v>
+      </c>
+      <c r="G32" s="31" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commiting library and text files -= MC
</commit_message>
<xml_diff>
--- a/library.xlsx
+++ b/library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Cividanes\Documents\Projects\Python\Dynamic-Story-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5148BE-8D20-4BAB-BE89-76057C4A5C1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC70E21-7FFC-4801-992C-9B4BBAD40A59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24210" windowHeight="9735" xr2:uid="{6E3BC6EE-222B-4AE7-8B06-6583935631F3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3581" uniqueCount="3142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3584" uniqueCount="3145">
   <si>
     <t xml:space="preserve">Valerius </t>
   </si>
@@ -10322,6 +10322,15 @@
   <si>
     <t xml:space="preserve">Crimson
 </t>
+  </si>
+  <si>
+    <t>Magister</t>
+  </si>
+  <si>
+    <t>Marhsall</t>
+  </si>
+  <si>
+    <t>Vizier</t>
   </si>
 </sst>
 </file>
@@ -11877,8 +11886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13EE33FA-8745-4FBA-A552-A58709A63450}">
   <dimension ref="A1:AC968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A278" sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -13396,6 +13405,9 @@
       <c r="C24" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="D24" s="1" t="s">
+        <v>3143</v>
+      </c>
       <c r="E24" s="17" t="s">
         <v>1040</v>
       </c>
@@ -13450,6 +13462,9 @@
       <c r="C25" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D25" s="5" t="s">
+        <v>3142</v>
+      </c>
       <c r="E25" s="17" t="s">
         <v>1041</v>
       </c>
@@ -13503,6 +13518,9 @@
       </c>
       <c r="C26" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>3144</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>1226</v>

</xml_diff>